<commit_message>
Started adding guard AI
Added a GuardSenses class, that can be used to create all kinds of guards, and a normal guard with some unfinished behavior
</commit_message>
<xml_diff>
--- a/RobotAndFrank/Documents/GuardBehaviors.xlsx
+++ b/RobotAndFrank/Documents/GuardBehaviors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ichsc\Desktop\Games\RobotAndFrank\RobotAndFrank\RobotAndFrank\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4B7390-9659-44F8-B928-ECEB2790592E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1005ABE4-E20E-45F2-9C6B-9EB71DFED53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,23 +440,23 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -480,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -491,7 +491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -499,7 +499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -510,7 +510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -518,7 +518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>